<commit_message>
minor corrections in README.md and added some references. Minor corrections in ProjectGantt.xlsx
</commit_message>
<xml_diff>
--- a/ProjectGantt.xlsx
+++ b/ProjectGantt.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Courses\ASDM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/livia/asdb_ass2/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -65,9 +71,6 @@
     <t>Gather images</t>
   </si>
   <si>
-    <t>Website class (jinja template, render)</t>
-  </si>
-  <si>
     <t>Interface with JavaScript</t>
   </si>
   <si>
@@ -80,9 +83,6 @@
     <t>Validating Route</t>
   </si>
   <si>
-    <t>Communication with stored procs</t>
-  </si>
-  <si>
     <t>Database class (connection, load data)</t>
   </si>
   <si>
@@ -116,9 +116,6 @@
     <t>Displaying success or fail</t>
   </si>
   <si>
-    <t>Animations (Lightening etc)</t>
-  </si>
-  <si>
     <t>Extra functionality</t>
   </si>
   <si>
@@ -198,12 +195,21 @@
   </si>
   <si>
     <t>Design</t>
+  </si>
+  <si>
+    <t>Animations (Lightning etc)</t>
+  </si>
+  <si>
+    <t>Communication with stored procedures</t>
+  </si>
+  <si>
+    <t>Website class (Jinja template, render)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -281,7 +287,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -291,7 +297,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -302,29 +308,29 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -656,150 +662,150 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB14" sqref="AB14"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="3" customWidth="1"/>
-    <col min="3" max="5" width="2.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" style="3" customWidth="1"/>
-    <col min="8" max="10" width="2.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="2.7109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" style="3" customWidth="1"/>
-    <col min="13" max="15" width="2.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="2.7109375" style="5" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="3" customWidth="1"/>
-    <col min="18" max="20" width="2.7109375" style="4" customWidth="1"/>
-    <col min="21" max="21" width="2.7109375" style="5" customWidth="1"/>
-    <col min="22" max="22" width="2.7109375" style="3" customWidth="1"/>
-    <col min="23" max="25" width="2.7109375" style="4" customWidth="1"/>
-    <col min="26" max="26" width="2.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" style="3" customWidth="1"/>
+    <col min="3" max="5" width="2.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" style="3" customWidth="1"/>
+    <col min="8" max="10" width="2.6640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="2.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" style="3" customWidth="1"/>
+    <col min="13" max="15" width="2.6640625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="2.6640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="3" customWidth="1"/>
+    <col min="18" max="20" width="2.6640625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="2.6640625" style="5" customWidth="1"/>
+    <col min="22" max="22" width="2.6640625" style="3" customWidth="1"/>
+    <col min="23" max="25" width="2.6640625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="2.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14"/>
       <c r="B1" s="15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="17"/>
       <c r="G1" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
       <c r="K1" s="17"/>
       <c r="L1" s="15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M1" s="16"/>
       <c r="N1" s="16"/>
       <c r="O1" s="16"/>
       <c r="P1" s="17"/>
       <c r="Q1" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R1" s="16"/>
       <c r="S1" s="16"/>
       <c r="T1" s="16"/>
       <c r="U1" s="17"/>
       <c r="V1" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="W1" s="16"/>
       <c r="X1" s="16"/>
       <c r="Y1" s="16"/>
       <c r="Z1" s="17"/>
     </row>
-    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>46</v>
-      </c>
       <c r="G2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>46</v>
-      </c>
       <c r="L2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>46</v>
-      </c>
       <c r="Q2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="S2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="T2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" s="20" t="s">
-        <v>46</v>
-      </c>
       <c r="V2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="W2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="X2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z2" s="20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="22"/>
@@ -827,31 +833,31 @@
       <c r="Y3" s="22"/>
       <c r="Z3" s="23"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F4" s="32"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P6" s="32"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="U7" s="32"/>
     </row>
-    <row r="8" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>0</v>
       </c>
@@ -881,7 +887,7 @@
       <c r="Y8" s="22"/>
       <c r="Z8" s="23"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -891,7 +897,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -899,7 +905,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -909,9 +915,9 @@
       <c r="E11" s="7"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="7"/>
@@ -919,7 +925,7 @@
       <c r="O12" s="7"/>
       <c r="P12" s="8"/>
     </row>
-    <row r="13" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>2</v>
       </c>
@@ -949,7 +955,7 @@
       <c r="Y13" s="22"/>
       <c r="Z13" s="23"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -959,7 +965,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -967,87 +973,87 @@
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="O22" s="7"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="7"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O23" s="10"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="9"/>
       <c r="R24" s="10"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="9"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="S26" s="7"/>
       <c r="T26" s="7"/>
       <c r="U26" s="8"/>
     </row>
-    <row r="27" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="28" t="s">
         <v>6</v>
       </c>
@@ -1077,9 +1083,9 @@
       <c r="Y27" s="22"/>
       <c r="Z27" s="23"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
@@ -1089,86 +1095,86 @@
       <c r="G28" s="6"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
       <c r="G30" s="9"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K32" s="8"/>
       <c r="L32" s="6"/>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K33" s="11"/>
       <c r="L33" s="9"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q35" s="6"/>
       <c r="R35" s="7"/>
       <c r="S35" s="7"/>
       <c r="T35" s="7"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q36" s="9"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R37" s="10"/>
       <c r="S37" s="10"/>
       <c r="T37" s="10"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R38" s="10"/>
       <c r="S38" s="10"/>
     </row>
-    <row r="39" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B39" s="21"/>
       <c r="C39" s="22"/>
@@ -1196,9 +1202,9 @@
       <c r="Y39" s="22"/>
       <c r="Z39" s="23"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
@@ -1208,94 +1214,94 @@
       <c r="G40" s="6"/>
       <c r="H40" s="7"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="11"/>
       <c r="G43" s="9"/>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K44" s="8"/>
       <c r="L44" s="6"/>
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K45" s="11"/>
       <c r="L45" s="9"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K46" s="11"/>
       <c r="L46" s="9"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M47" s="10"/>
       <c r="N47" s="10"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q48" s="6"/>
       <c r="R48" s="7"/>
       <c r="S48" s="7"/>
       <c r="T48" s="7"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q49" s="9"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R50" s="10"/>
       <c r="S50" s="10"/>
       <c r="T50" s="10"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R51" s="10"/>
       <c r="S51" s="10"/>
     </row>
-    <row r="52" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="22"/>
@@ -1323,37 +1329,37 @@
       <c r="Y52" s="22"/>
       <c r="Z52" s="23"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I53" s="24"/>
       <c r="J53" s="24"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="O54" s="24"/>
       <c r="P54" s="25"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O55" s="24"/>
       <c r="P55" s="25"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="U56" s="25"/>
       <c r="V56" s="26"/>
     </row>
-    <row r="57" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="28" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="22"/>
@@ -1381,9 +1387,9 @@
       <c r="Y57" s="22"/>
       <c r="Z57" s="23"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="Q58" s="29"/>
       <c r="R58" s="30"/>
@@ -1391,9 +1397,9 @@
       <c r="T58" s="30"/>
       <c r="U58" s="31"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="S59" s="30"/>
       <c r="T59" s="30"/>

</xml_diff>

<commit_message>
updated for sunday 28th jan
</commit_message>
<xml_diff>
--- a/ProjectGantt.xlsx
+++ b/ProjectGantt.xlsx
@@ -2,18 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\Martin\Courses\ASDM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1783947\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Gantt" sheetId="1" r:id="rId1"/>
+    <sheet name="Weekly" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="94">
   <si>
     <t>Architecture</t>
   </si>
@@ -204,9 +204,6 @@
     <t>Website class (Jinja template, render)</t>
   </si>
   <si>
-    <t>Explore Ajax/Python/parameters</t>
-  </si>
-  <si>
     <t>Website Framework</t>
   </si>
   <si>
@@ -219,27 +216,12 @@
     <t>Jinja template - basic html</t>
   </si>
   <si>
-    <t>Contains rect, pics, boat</t>
-  </si>
-  <si>
-    <t>Render method - generate the SVG html</t>
-  </si>
-  <si>
-    <t>Add to render all special effects</t>
-  </si>
-  <si>
     <t>Display Task</t>
   </si>
   <si>
     <t>Framework Task</t>
   </si>
   <si>
-    <t>Boat moving - hard coded route</t>
-  </si>
-  <si>
-    <t>Create simple Level class - hard coded</t>
-  </si>
-  <si>
     <t>Permission shared area</t>
   </si>
   <si>
@@ -253,12 +235,87 @@
   </si>
   <si>
     <t>Experiment Annimations, moving, lightning,explosion</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>Setup in own area</t>
+  </si>
+  <si>
+    <t>CC/LV</t>
+  </si>
+  <si>
+    <t>polygon</t>
+  </si>
+  <si>
+    <t>sea</t>
+  </si>
+  <si>
+    <t>lightning</t>
+  </si>
+  <si>
+    <t>grid</t>
+  </si>
+  <si>
+    <t>Move boat hardcoded path</t>
+  </si>
+  <si>
+    <t>Boat</t>
+  </si>
+  <si>
+    <t>Animations</t>
+  </si>
+  <si>
+    <t>Build SVG output in level class (hard code)</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Explore Ajax/Python/parameters/move class</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t>Create db</t>
+  </si>
+  <si>
+    <t>wire up db</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>html template</t>
+  </si>
+  <si>
+    <t>js/forms</t>
+  </si>
+  <si>
+    <t>booty</t>
+  </si>
+  <si>
+    <t>island image</t>
+  </si>
+  <si>
+    <t>Abstract svg logic in to level and obstacles</t>
+  </si>
+  <si>
+    <t>Moving stored procs and validations</t>
+  </si>
+  <si>
+    <t>game workflow</t>
+  </si>
+  <si>
+    <t>LV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -711,8 +768,8 @@
   <dimension ref="A1:Z59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,11 +998,11 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1149,9 +1206,9 @@
       <c r="A29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
@@ -1464,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C17"/>
+  <dimension ref="B1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,102 +1532,220 @@
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C1" s="33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F1" s="33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>61</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>70</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>